<commit_message>
task 4.2 and 4.3 finished
</commit_message>
<xml_diff>
--- a/submission_22_05_08_stock_chandla_motz/Schalttabelle.xlsx
+++ b/submission_22_05_08_stock_chandla_motz/Schalttabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJEKTE\ehp22\submission_22_05_08_stock_chandla_motz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A0C3E9-BDBB-4A35-9824-A5431627F406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61859E06-968F-40FD-8BDC-2B2E41F97F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{116D8E72-ADFC-4CB6-AE6A-17E35DFC4D65}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{116D8E72-ADFC-4CB6-AE6A-17E35DFC4D65}"/>
   </bookViews>
   <sheets>
     <sheet name="Fair Coffee Machine" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,6 +565,48 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -574,13 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -589,41 +625,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7C5ACE-6940-4BC2-93EB-93229F050524}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1006,47 +1009,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54" t="s">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="G1" s="61"/>
+      <c r="H1" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="53" t="s">
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="63" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="12"/>
-      <c r="O1" s="55" t="s">
+      <c r="O1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="50" t="s">
+      <c r="P1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="66" t="s">
         <v>12</v>
       </c>
       <c r="S1" s="24"/>
       <c r="T1" s="32"/>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="66" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1084,18 +1087,18 @@
       <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="52"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="66"/>
       <c r="S2" s="24"/>
       <c r="T2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="52"/>
+      <c r="U2" s="66"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
@@ -1910,17 +1913,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:K12 A17:K23 B13:K16 A27:A30">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -1939,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4232E49-CDAD-475F-A07E-5021AB86DA6D}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M16" sqref="A1:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1965,53 +1968,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54" t="s">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54" t="s">
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54" t="s">
+      <c r="H1" s="61"/>
+      <c r="I1" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="63" t="s">
         <v>18</v>
       </c>
       <c r="Q1" s="12"/>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="58" t="s">
+      <c r="U1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="56" t="s">
+      <c r="V1" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="52" t="s">
+      <c r="W1" s="52"/>
+      <c r="X1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="66" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2055,19 +2060,17 @@
       <c r="M2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
       <c r="Q2" s="12"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="52"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="66"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
@@ -2133,11 +2136,11 @@
         <f>IF(L3=1,_xlfn.TEXTJOIN(" * ",FALSE,O3,P3),"")</f>
         <v/>
       </c>
-      <c r="V3" s="60" t="str">
+      <c r="V3" s="51" t="str">
         <f>IF(M3=1,_xlfn.TEXTJOIN(" * ",FALSE,O3,P3),"")</f>
         <v/>
       </c>
-      <c r="W3" s="62"/>
+      <c r="W3" s="53"/>
       <c r="X3" s="37" t="str">
         <f>IF(G3=1,_xlfn.TEXTJOIN(" * ",FALSE,O3,P3),"")</f>
         <v/>
@@ -2211,11 +2214,11 @@
         <f t="shared" ref="U4:U17" si="4">IF(L4=1,_xlfn.TEXTJOIN(" * ",FALSE,O4,P4),"")</f>
         <v/>
       </c>
-      <c r="V4" s="60" t="str">
+      <c r="V4" s="51" t="str">
         <f t="shared" ref="V4:V17" si="5">IF(M4=1,_xlfn.TEXTJOIN(" * ",FALSE,O4,P4),"")</f>
         <v/>
       </c>
-      <c r="W4" s="62"/>
+      <c r="W4" s="53"/>
       <c r="X4" s="37" t="str">
         <f t="shared" ref="X4:X17" si="6">IF(G4=1,_xlfn.TEXTJOIN(" * ",FALSE,O4,P4),"")</f>
         <v/>
@@ -2289,11 +2292,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V5" s="60" t="str">
+      <c r="V5" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W5" s="62"/>
+      <c r="W5" s="53"/>
       <c r="X5" s="37" t="str">
         <f t="shared" si="6"/>
         <v>!S1 * S0 * A</v>
@@ -2367,11 +2370,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V6" s="60" t="str">
+      <c r="V6" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W6" s="62"/>
+      <c r="W6" s="53"/>
       <c r="X6" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2445,11 +2448,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V7" s="60" t="str">
+      <c r="V7" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W7" s="62"/>
+      <c r="W7" s="53"/>
       <c r="X7" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2523,11 +2526,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V8" s="60" t="str">
+      <c r="V8" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W8" s="62"/>
+      <c r="W8" s="53"/>
       <c r="X8" s="37" t="str">
         <f t="shared" si="6"/>
         <v>S1 * !S0 * A</v>
@@ -2601,11 +2604,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V9" s="60" t="str">
+      <c r="V9" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W9" s="62"/>
+      <c r="W9" s="53"/>
       <c r="X9" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2678,11 +2681,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V10" s="60" t="str">
+      <c r="V10" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W10" s="62"/>
+      <c r="W10" s="53"/>
       <c r="X10" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2756,11 +2759,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V11" s="60" t="str">
+      <c r="V11" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W11" s="62"/>
+      <c r="W11" s="53"/>
       <c r="X11" s="37" t="str">
         <f t="shared" si="6"/>
         <v>S1 * !S0 * !A * !B1 * !B2</v>
@@ -2834,11 +2837,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V12" s="60" t="str">
+      <c r="V12" s="51" t="str">
         <f t="shared" si="5"/>
         <v>S1 * S0 * A</v>
       </c>
-      <c r="W12" s="62"/>
+      <c r="W12" s="53"/>
       <c r="X12" s="37" t="str">
         <f t="shared" si="6"/>
         <v>S1 * S0 * A</v>
@@ -2912,11 +2915,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V13" s="60" t="str">
+      <c r="V13" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W13" s="62"/>
+      <c r="W13" s="53"/>
       <c r="X13" s="37" t="str">
         <f t="shared" si="6"/>
         <v>S1 * S0 * !A * B1 * !B2 * !B3</v>
@@ -2971,7 +2974,7 @@
         <v>28</v>
       </c>
       <c r="P14" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(IF(C14=1,"A","!A"),IF(D14&lt;&gt;"X", _xlfn.TEXTJOIN("",TRUE, " * ", IF(D14=1,"B1","!B1")),""),IF(E14&lt;&gt;"X", _xlfn.TEXTJOIN("",TRUE, " * ", IF(E14=1,"B2","!B2")),""),IF(F14&lt;&gt;"X", _xlfn.TEXTJOIN("",TRUE, " * ", IF(F14=1,"B3","!B3")),""))</f>
         <v>!A * B2 * !B3</v>
       </c>
       <c r="R14" s="37" t="str">
@@ -2990,11 +2993,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V14" s="60" t="str">
+      <c r="V14" s="51" t="str">
         <f>IF(M14=1,_xlfn.TEXTJOIN(" * ",FALSE,O14,P14),"")</f>
         <v/>
       </c>
-      <c r="W14" s="62"/>
+      <c r="W14" s="53"/>
       <c r="X14" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3068,11 +3071,11 @@
         <f t="shared" si="4"/>
         <v>S1 * S0 * !A * B3</v>
       </c>
-      <c r="V15" s="60" t="str">
+      <c r="V15" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W15" s="62"/>
+      <c r="W15" s="53"/>
       <c r="X15" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3146,11 +3149,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V16" s="60" t="str">
+      <c r="V16" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W16" s="62"/>
+      <c r="W16" s="53"/>
       <c r="X16" s="37" t="str">
         <f>IF(G16=1,_xlfn.TEXTJOIN(" * ",FALSE,O16,P16),"")</f>
         <v>S1 * S0 * !A * !B1 * !B2 * !B3</v>
@@ -3198,15 +3201,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="U17" s="59" t="str">
+      <c r="U17" s="50" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V17" s="60" t="str">
+      <c r="V17" s="51" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W17" s="62"/>
+      <c r="W17" s="53"/>
       <c r="X17" s="48" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3234,32 +3237,32 @@
       <c r="Q18" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="R18" s="63" t="str">
+      <c r="R18" s="54" t="str">
         <f>_xlfn.TEXTJOIN(" + ",TRUE,R3:R17)</f>
         <v>!S1 * S0 * A + !S1 * S0 * !A * !B1 + S1 * !S0 * A + S1 * !S0 * !A * B1 * !B2 + S1 * !S0 * !A * !B1 * !B2 + S1 * S0 * A + S1 * S0 * !A * B1 * !B2 * !B3 + S1 * S0 * !A * B2 * !B3 + S1 * S0 * !A * !B1 * !B2 * !B3</v>
       </c>
-      <c r="S18" s="64" t="str">
+      <c r="S18" s="55" t="str">
         <f>_xlfn.TEXTJOIN(" + ",TRUE,S3:S17)</f>
         <v>!S1 * S0 * !A * B1 + S1 * !S0 * !A * B1 * !B2 + S1 * S0 * !A * B1 * !B2 * !B3</v>
       </c>
-      <c r="T18" s="65" t="str">
+      <c r="T18" s="56" t="str">
         <f>_xlfn.TEXTJOIN(" + ",TRUE,T3:T17)</f>
         <v>S1 * !S0 * !A * B2 + S1 * S0 * !A * B2 * !B3</v>
       </c>
-      <c r="U18" s="66" t="str">
+      <c r="U18" s="57" t="str">
         <f>_xlfn.TEXTJOIN(" + ",TRUE,U3:U17)</f>
         <v>S1 * S0 * !A * B3</v>
       </c>
-      <c r="V18" s="67" t="str">
+      <c r="V18" s="58" t="str">
         <f>_xlfn.TEXTJOIN(" + ",TRUE,V3:V17)</f>
         <v>S1 * S0 * A</v>
       </c>
-      <c r="W18" s="68"/>
-      <c r="X18" s="63" t="str">
+      <c r="W18" s="59"/>
+      <c r="X18" s="54" t="str">
         <f>_xlfn.TEXTJOIN(" + ",TRUE,X3:X17)</f>
         <v>!S1 * S0 * A + S1 * !S0 * A + S1 * !S0 * !A * !B1 * !B2 + S1 * S0 * A + S1 * S0 * !A * B1 * !B2 * !B3 + S1 * S0 * !A * !B1 * !B2 * !B3</v>
       </c>
-      <c r="Y18" s="69" t="str">
+      <c r="Y18" s="60" t="str">
         <f>_xlfn.TEXTJOIN(" + ",TRUE,Y3:Y17)</f>
         <v>!S1 * !S0 * A + !S1 * S0 * !A * !B1 + S1 * !S0 * A + S1 * !S0 * !A * B1 * !B2 + S1 * S0 * A + S1 * S0 * !A * B2 * !B3 + S1 * S0 * !A * !B1 * !B2 * !B3</v>
       </c>
@@ -3405,19 +3408,20 @@
       <c r="K32" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="V1:V2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="A27:A31 A13:N23 A3:M12 K26:K32 L26:N28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>